<commit_message>
running for 100 iterations
</commit_message>
<xml_diff>
--- a/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
+++ b/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
@@ -493,152 +493,154 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', None), ('selector', None),
+          <t>Pipeline(steps=[('scaler', RobustScaler()), ('selector', 'passthrough'),
                 ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(criterion='entropy',
-                                                                     max_depth=6,
-                                                                     max_features='sqrt',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                     criterion='entropy',
+                                                                     max_depth=1,
+                                                                     max_features='log2',
+                                                                     min_samples_leaf=3,
+                                                                     min_samples_split=4,
+                                                                     random_state=42),
+                                    n_estimators=5, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.6476190476190476</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'scaler': RobustScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4285714285714285</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[1 0 0 1 0 0 1 1 0 1 0 0]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[0 1 1 0 1 1 1 1 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9767619047619047</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.003727604351283464</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5495238095238095</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.07485113344482791</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', StandardScaler()), ('selector', 'passthrough'),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                     max_depth=5,
+                                                                     max_features='log2',
                                                                      min_samples_leaf=2,
                                                                      min_samples_split=4,
                                                                      random_state=42),
-                                    n_estimators=5, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.7272262858469756</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{'selector': None, 'scaler': None, 'model__n_estimators': 5, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': None}</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.6250000000000001</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>[0 1 0 1 1 1 1 1 0 0 1 0]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>[1 1 0 0 1 0 1 1 1 1 1 1]</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.9768699705584745</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.005407720116491705</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.6019687785976815</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.08903405946696642</v>
+                                    n_estimators=10, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'scaler': StandardScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4285714285714285</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[1 0 1 0 0 0 0 1 1 0 1 1]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[0 1 0 1 1 0 1 1 1 1 0 1]</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9733809523809523</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.004983754460820096</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.5329523809523808</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.07454269106152089</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()), ('selector', None),
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', RobustScaler()), ('selector', 'passthrough'),
                 ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=5,
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=4,
                                                                      max_features='log2',
                                                                      min_samples_leaf=5,
                                                                      min_samples_split=6,
                                                                      random_state=42),
-                                    n_estimators=10, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.7233041841362198</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{'selector': None, 'scaler': StandardScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.6250000000000001</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>[0 0 1 1 0 0 1 1 1 0 1 1]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[1 1 1 1 1 1 1 1 0 0 0 1]</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.9795464222531121</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.004678107565998293</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.6030613955051554</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.0764568065265797</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()), ('selector', None),
-                ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=5,
-                                                                     max_features='sqrt',
-                                                                     min_samples_leaf=2,
-                                                                     min_samples_split=1,
-                                                                     random_state=42),
-                                    random_state=42))])</t>
+                                    n_estimators=5, random_state=42))])</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.729648148148148</v>
+        <v>0.6</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'selector': None, 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 1, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
+          <t>{'scaler': RobustScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[1 0 0 0 1 0 1 0 1 1 1 1]</t>
+          <t>[1 0 1 1 1 1 0 1 0 1 0 1]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[1 0 1 1 1 1 0 0 0 1 1 1]</t>
+          <t>[0 0 0 1 1 1 1 0 1 1 1 0]</t>
         </is>
       </c>
       <c r="G4" t="n">
         <v>42</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9737790783733475</v>
+        <v>0.983952380952381</v>
       </c>
       <c r="I4" t="n">
-        <v>0.00537000779414273</v>
+        <v>0.003776593048049497</v>
       </c>
       <c r="J4" t="n">
-        <v>0.616686254316408</v>
+        <v>0.4895238095238096</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0924237071027544</v>
+        <v>0.08853720127267714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
features selection, 5 runs
</commit_message>
<xml_diff>
--- a/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
+++ b/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,154 +493,259 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', RobustScaler()), ('selector', 'passthrough'),
+          <t>Pipeline(steps=[('scaler', RobustScaler()), ('selector', None),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                     max_depth=4,
+                                                                     max_features='log2',
+                                                                     min_samples_leaf=5,
+                                                                     min_samples_split=5,
+                                                                     random_state=42),
+                                    n_estimators=5, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.6380952380952382</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'selector': None, 'scaler': RobustScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4615384615384615</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[1 1 0 0 1 0 0 0 0 1 0 1]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[1 0 1 0 1 1 1 0 1 0 1 1]</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>77</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9633514165159734</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.00745717956232927</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5609403254972876</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.07283008747327888</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', StandardScaler()),
+                ('selector',
+                 SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1',
+                                                     random_state=42))),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=3,
+                                                                     min_samples_leaf=2,
+                                                                     min_samples_split=3,
+                                                                     random_state=42),
+                                    n_estimators=10, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'selector': SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1', random_state=42)), 'scaler': StandardScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 3, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': None, 'model__estimator__max_depth': 3, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4615384615384615</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[1 1 0 1 0 0 1 0 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[1 0 1 0 0 1 0 0 0 1 1 1]</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>69</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9733709273182958</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.006261276851512222</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.4958646616541353</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.09385801248311917</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', StandardScaler()), ('selector', None),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
                                                                      criterion='entropy',
-                                                                     max_depth=1,
-                                                                     max_features='log2',
+                                                                     max_depth=2,
+                                                                     max_features='sqrt',
+                                                                     min_samples_leaf=5,
+                                                                     min_samples_split=3,
+                                                                     random_state=42),
+                                    n_estimators=10, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'selector': None, 'scaler': StandardScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 3, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[1 0 1 1 1 1 0 1 0 1 0 1]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[1 0 0 1 0 0 0 0 0 1 0 1]</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>42</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9747685185185185</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.005562385210403438</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.5050264550264552</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.08440106424472506</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()), ('selector', None),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                     max_depth=5,
+                                                                     min_samples_leaf=5,
+                                                                     min_samples_split=6,
+                                                                     random_state=42),
+                                    n_estimators=10, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6380952380952382</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'selector': None, 'scaler': MinMaxScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': None, 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>[1 1 0 0 0 0 1 0 1 1 1 1]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>[1 1 0 0 0 1 1 1 1 0 1 1]</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>11</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9753968253968255</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.005918133544054688</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.502527924750147</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.07500704372350613</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
+                ('selector',
+                 SelectFromModel(estimator=ExtraTreesClassifier(random_state=42))),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(criterion='entropy',
+                                                                     max_depth=6,
+                                                                     max_features='sqrt',
                                                                      min_samples_leaf=3,
                                                                      min_samples_split=4,
                                                                      random_state=42),
-                                    n_estimators=5, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.6476190476190476</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{'scaler': RobustScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>[1 0 0 1 0 0 1 1 0 1 0 0]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>[0 1 1 0 1 1 1 1 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.9767619047619047</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.003727604351283464</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.5495238095238095</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.07485113344482791</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()), ('selector', 'passthrough'),
-                ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     max_depth=5,
-                                                                     max_features='log2',
-                                                                     min_samples_leaf=2,
-                                                                     min_samples_split=4,
-                                                                     random_state=42),
                                     n_estimators=10, random_state=42))])</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>0.6190476190476191</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{'scaler': StandardScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>[1 0 1 0 0 0 0 1 1 0 1 1]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[0 1 0 1 1 0 1 1 1 1 0 1]</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.9733809523809523</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.004983754460820096</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.5329523809523808</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.07454269106152089</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', RobustScaler()), ('selector', 'passthrough'),
-                ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=4,
-                                                                     max_features='log2',
-                                                                     min_samples_leaf=5,
-                                                                     min_samples_split=6,
-                                                                     random_state=42),
-                                    n_estimators=5, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{'scaler': RobustScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.5333333333333333</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>[1 0 1 1 1 1 0 1 0 1 0 1]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[0 0 0 1 1 1 1 0 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>42</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.983952380952381</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.003776593048049497</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.4895238095238096</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.08853720127267714</v>
+      <c r="B6" t="n">
+        <v>0.6095238095238095</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'selector': SelectFromModel(estimator=ExtraTreesClassifier(random_state=42)), 'scaler': MinMaxScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': None}</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5714285714285715</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[1 1 1 1 0 0 0 0 1 1 0 0]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[1 1 1 0 1 1 1 1 1 0 0 0]</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>14</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.9544679600235156</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.008827083274573471</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5188712522045855</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.08442370963591503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
linear tree and linear boost
</commit_message>
<xml_diff>
--- a/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
+++ b/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
@@ -531,16 +531,16 @@
         <v>42</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9735986487458891</v>
+        <v>0.9706992789427162</v>
       </c>
       <c r="I2" t="n">
-        <v>0.006924392007874155</v>
+        <v>0.007943953096139331</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5152114032935111</v>
+        <v>0.5185769661710837</v>
       </c>
       <c r="K2" t="n">
-        <v>0.153423826004206</v>
+        <v>0.1538086624801142</v>
       </c>
     </row>
     <row r="3">
@@ -548,28 +548,26 @@
         <is>
           <t>Pipeline(steps=[('scaler', RobustScaler()),
                 ('selector',
-                 SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1',
-                                                     random_state=42))),
+                 &lt;__main__.NamedFeatureSelector object at 0x7f91c9d63760&gt;),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     max_depth=5,
+                                                                     max_depth=6,
                                                                      max_features='sqrt',
-                                                                     min_samples_leaf=2,
-                                                                     min_samples_split=6,
+                                                                     min_samples_split=4,
                                                                      random_state=42),
                                     n_estimators=10, random_state=42))])</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6850732600732601</v>
+        <v>0.699871794871795</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'selector': SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1', random_state=42)), 'scaler': RobustScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f91243515b0&gt;, 'scaler': RobustScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 1, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.75</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -578,49 +576,49 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[0 0 0 1 1 1 1 1 1 1 0 0]</t>
+          <t>[0 1 1 1 1 0 1 1 1 1 1 0]</t>
         </is>
       </c>
       <c r="G3" t="n">
         <v>69</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9746549119932693</v>
+        <v>0.9724702579371853</v>
       </c>
       <c r="I3" t="n">
-        <v>0.006903994691276204</v>
+        <v>0.007081119230557222</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5909617014822124</v>
+        <v>0.6025795465971937</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1249955144267885</v>
+        <v>0.1234478071525753</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
                 ('selector',
-                 SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1',
-                                                     random_state=42))),
+                 &lt;__main__.NamedFeatureSelector object at 0x7f91c7468e80&gt;),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=6,
-                                                                     min_samples_leaf=3,
+                                                                     min_samples_leaf=5,
+                                                                     min_samples_split=6,
                                                                      random_state=42),
                                     random_state=42))])</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7022408963585434</v>
+        <v>0.7034523809523809</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'selector': SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1', random_state=42)), 'scaler': StandardScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 2, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': None, 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
+          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f9124366970&gt;, 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': None, 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.823529411764706</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -629,23 +627,23 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[0 1 1 1 0 1 1 1 1 1 1 0]</t>
+          <t>[0 1 1 0 0 1 0 1 1 0 0 0]</t>
         </is>
       </c>
       <c r="G4" t="n">
         <v>23</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9749427130333268</v>
+        <v>0.9739405914781303</v>
       </c>
       <c r="I4" t="n">
-        <v>0.005727034483929828</v>
+        <v>0.006152057408022343</v>
       </c>
       <c r="J4" t="n">
-        <v>0.6027200692911788</v>
+        <v>0.6035929364752894</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1270955716110641</v>
+        <v>0.1268847575029185</v>
       </c>
     </row>
     <row r="5">
@@ -688,16 +686,16 @@
         <v>99</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9838732934144306</v>
+        <v>0.9753857809243834</v>
       </c>
       <c r="I5" t="n">
-        <v>0.004036074382988982</v>
+        <v>0.005251340185646229</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6003637668248059</v>
+        <v>0.6038589580354286</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1360021381544983</v>
+        <v>0.1390832661757343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switching to try 70/30 and 80/20 split
</commit_message>
<xml_diff>
--- a/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
+++ b/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
@@ -494,183 +494,182 @@
       <c r="A2" t="inlineStr">
         <is>
           <t>Pipeline(steps=[('scaler', RobustScaler()),
-                ('selector',
-                 SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1',
-                                                     random_state=42))),
+                ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                     criterion='entropy',
                                                                      max_depth=5,
-                                                                     min_samples_leaf=2,
+                                                                     max_features='sqrt',
+                                                                     min_samples_leaf=6,
+                                                                     min_samples_split=6,
+                                                                     random_state=42),
+                                    random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5416028416028416</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': RobustScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 6, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[1 0 1 1 1 1 0 1 0 1 0 1]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[1 0 1 1 1 1 0 0 1 0 0 1]</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>42</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.9006177907956395</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.02356486820354882</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.4554321123321124</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.1668581131322856</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', RobustScaler()),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=4,
+                                                                     max_features='sqrt',
+                                                                     min_samples_leaf=4,
                                                                      min_samples_split=5,
                                                                      random_state=42),
                                     n_estimators=10, random_state=42))])</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0.6416749916749916</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{'selector': SelectFromModel(estimator=LinearSVC(dual=False, penalty='l1', random_state=42)), 'scaler': RobustScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': None, 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.823529411764706</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>[1 0 1 1 1 1 0 1 0 1 0 1]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>[1 1 1 1 1 1 0 0 1 1 0 1]</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>42</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.9706992789427162</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.007943953096139331</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.5185769661710837</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.1538086624801142</v>
+      <c r="B3" t="n">
+        <v>0.631068931068931</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': RobustScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[1 1 0 1 0 0 1 0 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[0 1 0 1 1 1 0 1 0 1 1 0]</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>69</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8908199617682057</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.02548209242292365</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.5392226218226218</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.1565767270107846</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', RobustScaler()),
-                ('selector',
-                 &lt;__main__.NamedFeatureSelector object at 0x7f91c9d63760&gt;),
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                     max_depth=6,
+                                                                     min_samples_leaf=6,
+                                                                     min_samples_split=6,
+                                                                     random_state=42),
+                                    n_estimators=5, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.6902219349278171</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 6, 'model__estimator__max_features': None, 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.4285714285714285</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[0 1 0 0 1 1 1 1 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[0 1 1 1 0 0 0 1 1 0 0 1]</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>23</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.910592479779327</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.02195213284173735</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.5409538262391203</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.1475826440591196</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
+                ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
                                                                      max_depth=6,
                                                                      max_features='sqrt',
+                                                                     min_samples_leaf=3,
                                                                      min_samples_split=4,
                                                                      random_state=42),
-                                    n_estimators=10, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.699871794871795</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f91243515b0&gt;, 'scaler': RobustScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 1, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>[1 1 0 1 0 0 1 0 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[0 1 1 1 1 0 1 1 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>69</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.9724702579371853</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.007081119230557222</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.6025795465971937</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.1234478071525753</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
-                ('selector',
-                 &lt;__main__.NamedFeatureSelector object at 0x7f91c7468e80&gt;),
-                ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=6,
-                                                                     min_samples_leaf=5,
-                                                                     min_samples_split=6,
-                                                                     random_state=42),
-                                    random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.7034523809523809</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{'selector': &lt;__main__.NamedFeatureSelector object at 0x7f9124366970&gt;, 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': None, 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.6153846153846154</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>[0 1 0 0 1 1 1 1 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[0 1 1 0 0 1 0 1 1 0 0 0]</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>23</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.9739405914781303</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.006152057408022343</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.6035929364752894</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1268847575029185</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', RobustScaler()), ('selector', None),
-                ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     criterion='entropy',
-                                                                     max_depth=6,
-                                                                     max_features='sqrt',
-                                                                     min_samples_leaf=3,
-                                                                     min_samples_split=6,
-                                                                     random_state=42),
-                                    random_state=42))])</t>
+                                    n_estimators=5, random_state=42))])</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7074096818214465</v>
+        <v>0.6918181818181818</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'selector': None, 'scaler': RobustScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8000000000000002</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -679,23 +678,23 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[1 1 1 1 0 1 0 1 1 1 1 1]</t>
+          <t>[0 1 1 0 0 1 0 0 0 1 1 0]</t>
         </is>
       </c>
       <c r="G5" t="n">
         <v>99</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9753857809243834</v>
+        <v>0.8738143952987326</v>
       </c>
       <c r="I5" t="n">
-        <v>0.005251340185646229</v>
+        <v>0.02355277637360543</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6038589580354286</v>
+        <v>0.5291931382343147</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1390832661757343</v>
+        <v>0.1640374644108655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
70/30 optimize precision and recall
</commit_message>
<xml_diff>
--- a/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
+++ b/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,106 +451,137 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Validation Score</t>
+          <t>CV Train F1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>CV Test F1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Validation F1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>CV Train Precision</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CV Test Precision</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Validation Precision</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>CV Train Recall</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>CV Test Recall</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Validation Recall</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Y Val (Validation)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Y Pred (Validation)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Seed</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>CV Train Mean</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>CV Train STD</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>CV Test Mean</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>CV Test STD</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', RobustScaler()),
+          <t>Pipeline(steps=[('scaler', None),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=2,
+                                                                     min_samples_leaf=2,
+                                                                     min_samples_split=5,
+                                                                     random_state=42),
+                                    n_estimators=5, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.6366666666666666</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': None, 'model__n_estimators': 5, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': None, 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9071927927573502</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.4258999167499167</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5853658536585366</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9922766962365251</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.4929436507936508</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.631578947368421</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8368809523809524</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.5454545454545454</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>[1 0 1 1 1 1 0 1 0 1 0 1 0 1 1 0 0 1 1 1 1 0 1 1 0 1 1 1 1 0 0 0 0 1 0 1]</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>[1 1 1 1 0 0 0 0 1 0 1 1 0 1 0 0 0 0 0 1 0 1 1 0 0 1 0 1 1 1 1 0 0 1 1 1]</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', StandardScaler()),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
                                                                      criterion='entropy',
-                                                                     max_depth=5,
-                                                                     max_features='sqrt',
-                                                                     min_samples_leaf=6,
-                                                                     min_samples_split=6,
-                                                                     random_state=42),
-                                    random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.5416028416028416</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': RobustScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 6, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.7999999999999999</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>[1 0 1 1 1 1 0 1 0 1 0 1]</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>[1 0 1 1 1 1 0 0 1 0 0 1]</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>42</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.9006177907956395</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.02356486820354882</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.4554321123321124</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.1668581131322856</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', RobustScaler()),
-                ('selector', RandomUnderSampler(random_state=42)),
-                ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=4,
-                                                                     max_features='sqrt',
+                                                                     max_depth=6,
+                                                                     max_features='log2',
                                                                      min_samples_leaf=4,
                                                                      min_samples_split=5,
                                                                      random_state=42),
@@ -558,143 +589,243 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.631068931068931</v>
+        <v>0.6421428571428571</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': RobustScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>[1 1 0 1 0 0 1 0 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[0 1 0 1 1 1 0 1 0 1 1 0]</t>
-        </is>
+        <v>0.9244231100188952</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.4704725996225997</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.7083333333333334</v>
       </c>
       <c r="G3" t="n">
+        <v>0.9882288499386802</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.5083718253968253</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.869575</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.466</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>[1 1 0 1 0 0 1 0 1 1 1 0 1 1 1 1 1 1 1 1 0 0 1 0 0 1 0 1 1 0 1 1 0 1 1 1]</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>[0 0 0 1 1 0 1 1 1 1 1 0 0 0 1 1 1 1 1 1 1 1 1 1 0 0 1 1 0 0 0 1 1 1 1 1]</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
         <v>69</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.8908199617682057</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.02548209242292365</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.5392226218226218</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.1565767270107846</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
+          <t>Pipeline(steps=[('scaler', StandardScaler()),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     max_depth=6,
-                                                                     min_samples_leaf=6,
+                                                                     max_depth=4,
+                                                                     max_features='sqrt',
+                                                                     min_samples_leaf=3,
+                                                                     min_samples_split=5,
+                                                                     random_state=42),
+                                    random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.6411904761904762</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9624787346737688</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.5166044899544899</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6382978723404256</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9902841487789916</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.5434972222222222</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9372894736842105</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.5204</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.5769230769230769</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>[0 1 0 0 1 1 1 1 1 1 1 0 1 1 1 1 1 1 1 1 0 1 1 1 0 1 0 1 0 1 0 1 1 1 0 1]</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>[1 1 1 0 0 1 0 1 1 1 1 0 0 0 1 0 0 0 1 0 1 0 1 1 1 1 0 1 1 1 0 0 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', StandardScaler()),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(criterion='entropy',
+                                                                     max_depth=2,
+                                                                     min_samples_leaf=3,
+                                                                     min_samples_split=5,
+                                                                     random_state=42),
+                                    n_estimators=5, random_state=42))])</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6278571428571429</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': None, 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': None}</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8906760046554379</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.4263956543456544</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9830304974795054</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.4890777777777778</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.816404761904762</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.4036</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.4090909090909091</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>[0 1 1 0 0 1 0 0 0 0 1 1 1 0 0 1 1 0 1 1 1 1 1 1 1 1 0 0 1 0 1 1 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>[0 0 1 0 1 1 0 1 1 1 1 1 0 0 1 0 1 1 0 0 0 1 1 0 1 0 1 1 0 1 0 0 0 1 0 0]</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pipeline(steps=[('scaler', None),
+                ('selector', RandomUnderSampler(random_state=42)),
+                ('model',
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
+                                                                     max_depth=2,
+                                                                     max_features='log2',
+                                                                     min_samples_leaf=5,
                                                                      min_samples_split=6,
                                                                      random_state=42),
                                     n_estimators=5, random_state=42))])</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.6902219349278171</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 6, 'model__estimator__max_features': None, 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>[0 1 0 0 1 1 1 1 1 1 1 0]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[0 1 1 1 0 0 0 1 1 0 0 1]</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>23</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.910592479779327</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.02195213284173735</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.5409538262391203</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1475826440591196</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
-                ('selector', RandomUnderSampler(random_state=42)),
-                ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     max_depth=6,
-                                                                     max_features='sqrt',
-                                                                     min_samples_leaf=3,
-                                                                     min_samples_split=4,
-                                                                     random_state=42),
-                                    n_estimators=5, random_state=42))])</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.6918181818181818</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8000000000000002</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>[0 1 1 0 0 1 0 0 0 0 1 1]</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>[0 1 1 0 0 1 0 0 0 1 1 0]</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>99</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.8738143952987326</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.02355277637360543</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.5291931382343147</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.1640374644108655</v>
+      <c r="B6" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': None, 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.8799915630104335</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5223221667221667</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5116279069767442</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.9850217542941452</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5782190476190475</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.4782608695652174</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.797</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5104000000000001</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>[1 0 1 1 0 0 0 0 1 0 1 1 0 1 1 0 1 0 0 0 0 0 1 1 1 0 1 0 1 1 1 1 1 1 1 0]</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>[1 0 1 1 1 1 1 1 0 0 0 1 1 1 1 1 0 1 0 1 1 1 1 1 0 1 1 1 0 1 0 1 0 0 0 0]</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
80/20 optimize precision and recall
</commit_message>
<xml_diff>
--- a/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
+++ b/results/AdaBoostClassifier_DecisionTreeClassifier.xlsx
@@ -513,59 +513,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', None),
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
-                 AdaBoostClassifier(estimator=DecisionTreeClassifier(max_depth=2,
-                                                                     min_samples_leaf=2,
-                                                                     min_samples_split=5,
+                 AdaBoostClassifier(estimator=DecisionTreeClassifier(criterion='entropy',
+                                                                     max_depth=5,
+                                                                     max_features='sqrt',
                                                                      random_state=42),
-                                    n_estimators=5, random_state=42))])</t>
+                                    n_estimators=10, random_state=42))])</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6366666666666666</v>
+        <v>0.6319580419580418</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': None, 'model__n_estimators': 5, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 2, 'model__estimator__max_features': None, 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': None}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 2, 'model__estimator__min_samples_leaf': 1, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': None}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.9071927927573502</v>
+        <v>0.9237305050552113</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4258999167499167</v>
+        <v>0.4737500444000445</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5853658536585366</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9922766962365251</v>
+        <v>0.9881859095293996</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4929436507936508</v>
+        <v>0.5311805555555555</v>
       </c>
       <c r="I2" t="n">
-        <v>0.631578947368421</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8368809523809524</v>
+        <v>0.8685106382978722</v>
       </c>
       <c r="K2" t="n">
-        <v>0.398</v>
+        <v>0.4490000000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.75</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[1 0 1 1 1 1 0 1 0 1 0 1 0 1 1 0 0 1 1 1 1 0 1 1 0 1 1 1 1 0 0 0 0 1 0 1]</t>
+          <t>[1 0 1 1 1 1 0 1 0 1 0 1 0 1 1 0 0 1 1 1 1 0 1 1]</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[1 1 1 1 0 0 0 0 1 0 1 1 0 1 0 0 0 0 0 1 0 1 1 0 0 1 0 1 1 1 1 0 0 1 1 1]</t>
+          <t>[1 0 1 1 1 1 1 0 1 1 1 1 1 0 1 0 0 1 0 1 1 1 1 0]</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -579,58 +579,56 @@
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     criterion='entropy',
-                                                                     max_depth=6,
-                                                                     max_features='log2',
-                                                                     min_samples_leaf=4,
-                                                                     min_samples_split=5,
+                                                                     max_depth=1,
+                                                                     max_features='sqrt',
+                                                                     min_samples_leaf=5,
                                                                      random_state=42),
-                                    n_estimators=10, random_state=42))])</t>
+                                    random_state=42))])</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6421428571428571</v>
+        <v>0.6254778554778554</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 4, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 6, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 2, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 1, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.9244231100188952</v>
+        <v>0.9149271946510816</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4704725996225997</v>
+        <v>0.4634015040515041</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9882288499386802</v>
+        <v>0.9842006407077476</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5083718253968253</v>
+        <v>0.5814345238095239</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="J3" t="n">
-        <v>0.869575</v>
+        <v>0.8564255319148937</v>
       </c>
       <c r="K3" t="n">
-        <v>0.466</v>
+        <v>0.4105</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7083333333333334</v>
+        <v>0.5625</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[1 1 0 1 0 0 1 0 1 1 1 0 1 1 1 1 1 1 1 1 0 0 1 0 0 1 0 1 1 0 1 1 0 1 1 1]</t>
+          <t>[1 1 0 1 0 0 1 0 1 1 1 0 1 1 1 1 1 1 1 1 0 0 1 0]</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>[0 0 0 1 1 0 1 1 1 1 1 0 0 0 1 1 1 1 1 1 1 1 1 1 0 0 1 1 0 0 0 1 1 1 1 1]</t>
+          <t>[0 1 1 1 1 0 0 0 1 1 0 0 1 0 1 1 1 1 0 0 1 0 0 1]</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -640,61 +638,62 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler', RobustScaler()),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     max_depth=4,
-                                                                     max_features='sqrt',
+                                                                     criterion='entropy',
+                                                                     max_depth=5,
+                                                                     max_features='log2',
                                                                      min_samples_leaf=3,
-                                                                     min_samples_split=5,
+                                                                     min_samples_split=4,
                                                                      random_state=42),
-                                    random_state=42))])</t>
+                                    n_estimators=5, random_state=42))])</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6411904761904762</v>
+        <v>0.6095959595959596</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 4, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': RobustScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 4, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.9624787346737688</v>
+        <v>0.9430558065748097</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5166044899544899</v>
+        <v>0.5020255855255855</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6382978723404256</v>
+        <v>0.5625</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9902841487789916</v>
+        <v>0.9872708877627798</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5434972222222222</v>
+        <v>0.5376944444444445</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9372894736842105</v>
+        <v>0.9036888888888889</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5204</v>
+        <v>0.4994000000000001</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5769230769230769</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>[0 1 0 0 1 1 1 1 1 1 1 0 1 1 1 1 1 1 1 1 0 1 1 1 0 1 0 1 0 1 0 1 1 1 0 1]</t>
+          <t>[0 1 0 0 1 1 1 1 1 1 1 0 1 1 1 1 1 1 1 1 0 1 1 1]</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>[1 1 1 0 0 1 0 1 1 1 1 0 0 0 1 0 0 0 1 0 1 0 1 1 1 1 0 1 1 1 0 0 1 1 1 0]</t>
+          <t>[0 0 1 1 0 1 0 1 0 0 1 1 0 0 1 1 1 1 1 0 1 1 0 0]</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -704,60 +703,59 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler', MinMaxScaler()),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(criterion='entropy',
-                                                                     max_depth=2,
-                                                                     min_samples_leaf=3,
-                                                                     min_samples_split=5,
+                                                                     max_depth=5,
+                                                                     min_samples_split=3,
                                                                      random_state=42),
-                                    n_estimators=5, random_state=42))])</t>
+                                    random_state=42))])</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6278571428571429</v>
+        <v>0.61993006993007</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__n_estimators': 5, 'model__estimator__min_samples_split': 5, 'model__estimator__min_samples_leaf': 3, 'model__estimator__max_features': None, 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': None}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': MinMaxScaler(), 'model__n_estimators': 50, 'model__estimator__min_samples_split': 3, 'model__estimator__min_samples_leaf': 1, 'model__estimator__max_features': None, 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'entropy', 'model__estimator__class_weight': None}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8906760046554379</v>
+        <v>0.888061214508038</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4263956543456544</v>
+        <v>0.4877457875457875</v>
       </c>
       <c r="F5" t="n">
-        <v>0.45</v>
+        <v>0.5925925925925927</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9830304974795054</v>
+        <v>0.9808044650995831</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4890777777777778</v>
+        <v>0.5589289682539682</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="J5" t="n">
-        <v>0.816404761904762</v>
+        <v>0.8133877551020408</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4036</v>
+        <v>0.4581666666666667</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4090909090909091</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>[0 1 1 0 0 1 0 0 0 0 1 1 1 0 0 1 1 0 1 1 1 1 1 1 1 1 0 0 1 0 1 1 1 1 1 0]</t>
+          <t>[0 1 1 0 0 1 0 0 0 0 1 1 1 0 0 1 1 0 1 1 1 1 1 1]</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>[0 0 1 0 1 1 0 1 1 1 1 1 0 0 1 0 1 1 0 0 0 1 1 0 1 0 1 1 0 1 0 0 0 1 0 0]</t>
+          <t>[1 1 1 1 1 0 0 1 0 0 1 0 0 0 1 1 0 0 0 1 0 1 1 1]</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -767,61 +765,61 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', None),
+          <t>Pipeline(steps=[('scaler', RobustScaler()),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  AdaBoostClassifier(estimator=DecisionTreeClassifier(class_weight='balanced',
-                                                                     max_depth=2,
-                                                                     max_features='log2',
-                                                                     min_samples_leaf=5,
+                                                                     max_depth=5,
+                                                                     max_features='sqrt',
+                                                                     min_samples_leaf=6,
                                                                      min_samples_split=6,
                                                                      random_state=42),
-                                    n_estimators=5, random_state=42))])</t>
+                                    n_estimators=10, random_state=42))])</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.72</v>
+        <v>0.6350793650793651</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': None, 'model__n_estimators': 5, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 5, 'model__estimator__max_features': 'log2', 'model__estimator__max_depth': 2, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': RobustScaler(), 'model__n_estimators': 10, 'model__estimator__min_samples_split': 6, 'model__estimator__min_samples_leaf': 6, 'model__estimator__max_features': 'sqrt', 'model__estimator__max_depth': 5, 'model__estimator__criterion': 'gini', 'model__estimator__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.8799915630104335</v>
+        <v>0.8699615838084128</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5223221667221667</v>
+        <v>0.5203073482073483</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5116279069767442</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9850217542941452</v>
+        <v>0.9834527463483009</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5782190476190475</v>
+        <v>0.6004416666666667</v>
       </c>
       <c r="I6" t="n">
-        <v>0.4782608695652174</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="J6" t="n">
-        <v>0.797</v>
+        <v>0.7821730769230767</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5104000000000001</v>
+        <v>0.4821666666666667</v>
       </c>
       <c r="L6" t="n">
-        <v>0.55</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>[1 0 1 1 0 0 0 0 1 0 1 1 0 1 1 0 1 0 0 0 0 0 1 1 1 0 1 0 1 1 1 1 1 1 1 0]</t>
+          <t>[1 0 1 1 0 0 0 0 1 0 1 1 0 1 1 0 1 0 0 0 0 0 1 1]</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>[1 0 1 1 1 1 1 1 0 0 0 1 1 1 1 1 0 1 0 1 1 1 1 1 0 1 1 1 0 1 0 1 0 0 0 0]</t>
+          <t>[1 0 0 0 0 1 0 0 0 1 1 0 1 0 0 1 1 1 1 0 1 0 1 0]</t>
         </is>
       </c>
       <c r="O6" t="n">

</xml_diff>